<commit_message>
Remove AppConfig and migrate database configuration to YAML
The `AppConfig` class was removed, and its database configuration was replaced with properties in `application.yaml` for better modularity and clarity. This also updates `.gitignore` to include `.gradle/` files and removes unused imports in `ExcelRunner.kt`.
</commit_message>
<xml_diff>
--- a/report-output.xlsx
+++ b/report-output.xlsx
@@ -44,6 +44,21 @@
     <t>Metrics</t>
   </si>
   <si>
+    <t>2025-05-24</t>
+  </si>
+  <si>
+    <t>2025-05-23</t>
+  </si>
+  <si>
+    <t>2025-05-22</t>
+  </si>
+  <si>
+    <t>2025-05-21</t>
+  </si>
+  <si>
+    <t>2025-05-20</t>
+  </si>
+  <si>
     <t>2025-05-19</t>
   </si>
   <si>
@@ -117,21 +132,6 @@
   </si>
   <si>
     <t>2025-04-25</t>
-  </si>
-  <si>
-    <t>2025-04-24</t>
-  </si>
-  <si>
-    <t>2025-04-23</t>
-  </si>
-  <si>
-    <t>2025-04-22</t>
-  </si>
-  <si>
-    <t>2025-04-21</t>
-  </si>
-  <si>
-    <t>2025-04-20</t>
   </si>
 </sst>
 </file>
@@ -540,7 +540,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>76.56961008800904</v>
+        <v>92.22734806402124</v>
       </c>
     </row>
     <row r="3">
@@ -548,7 +548,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n" s="0">
-        <v>40.609384897677906</v>
+        <v>15.856837896144981</v>
       </c>
     </row>
     <row r="4">
@@ -556,7 +556,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n" s="0">
-        <v>49.136278065637086</v>
+        <v>71.0903809450719</v>
       </c>
     </row>
     <row r="5">
@@ -564,7 +564,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n" s="0">
-        <v>14.510562106714298</v>
+        <v>68.72211276804812</v>
       </c>
     </row>
     <row r="6">
@@ -572,7 +572,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n" s="0">
-        <v>36.866494246558126</v>
+        <v>9.254602841671488</v>
       </c>
     </row>
     <row r="7">
@@ -580,7 +580,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n" s="0">
-        <v>49.52513185026752</v>
+        <v>64.18599413793459</v>
       </c>
     </row>
     <row r="8">
@@ -588,7 +588,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n" s="0">
-        <v>2.8902165972525706</v>
+        <v>93.31987493146613</v>
       </c>
     </row>
     <row r="9">
@@ -596,7 +596,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n" s="0">
-        <v>6.165738530591003</v>
+        <v>92.85739095585566</v>
       </c>
     </row>
     <row r="10">
@@ -604,7 +604,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="n" s="0">
-        <v>5.043628635339747</v>
+        <v>12.602063892186177</v>
       </c>
     </row>
     <row r="11">
@@ -612,7 +612,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="n" s="0">
-        <v>54.92116434265919</v>
+        <v>44.669219955222</v>
       </c>
     </row>
     <row r="12">
@@ -620,7 +620,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="n" s="0">
-        <v>68.14365927592549</v>
+        <v>96.63287027506601</v>
       </c>
     </row>
     <row r="13">
@@ -628,7 +628,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="n" s="0">
-        <v>61.8821640865313</v>
+        <v>40.58446468419671</v>
       </c>
     </row>
     <row r="14">
@@ -636,7 +636,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="n" s="0">
-        <v>42.7822863352987</v>
+        <v>10.733536532579013</v>
       </c>
     </row>
     <row r="15">
@@ -644,7 +644,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="n" s="0">
-        <v>7.897211819884687</v>
+        <v>20.48577887214841</v>
       </c>
     </row>
     <row r="16">
@@ -652,7 +652,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="n" s="0">
-        <v>89.51445875953962</v>
+        <v>8.0225586267054</v>
       </c>
     </row>
     <row r="17">
@@ -660,7 +660,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="n" s="0">
-        <v>78.01660765380396</v>
+        <v>57.415730786410236</v>
       </c>
     </row>
     <row r="18">
@@ -668,7 +668,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="n" s="0">
-        <v>58.72117646828251</v>
+        <v>41.158514962576675</v>
       </c>
     </row>
     <row r="19">
@@ -676,7 +676,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="n" s="0">
-        <v>49.31655378526841</v>
+        <v>93.85877590125692</v>
       </c>
     </row>
     <row r="20">
@@ -684,7 +684,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="n" s="0">
-        <v>6.747530563921689</v>
+        <v>24.229812416790786</v>
       </c>
     </row>
     <row r="21">
@@ -692,7 +692,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="n" s="0">
-        <v>95.20476088248073</v>
+        <v>81.01886898305807</v>
       </c>
     </row>
     <row r="22">
@@ -700,7 +700,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="n" s="0">
-        <v>3.7760648279025144</v>
+        <v>21.140750912515372</v>
       </c>
     </row>
     <row r="23">
@@ -708,7 +708,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="n" s="0">
-        <v>56.03952378547119</v>
+        <v>57.294525188168734</v>
       </c>
     </row>
     <row r="24">
@@ -716,7 +716,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="n" s="0">
-        <v>53.76078465239241</v>
+        <v>95.22876365628775</v>
       </c>
     </row>
     <row r="25">
@@ -724,7 +724,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="n" s="0">
-        <v>63.95278797259271</v>
+        <v>88.97246215136958</v>
       </c>
     </row>
     <row r="26">
@@ -732,7 +732,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="n" s="0">
-        <v>73.81388027898994</v>
+        <v>35.11854227313118</v>
       </c>
     </row>
     <row r="27">
@@ -740,7 +740,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="n" s="0">
-        <v>26.303164067992434</v>
+        <v>40.04282223732667</v>
       </c>
     </row>
     <row r="28">
@@ -748,7 +748,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="n" s="0">
-        <v>65.04040275523835</v>
+        <v>14.4887007107815</v>
       </c>
     </row>
     <row r="29">
@@ -756,7 +756,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="n" s="0">
-        <v>84.98212973509615</v>
+        <v>46.74362776943893</v>
       </c>
     </row>
     <row r="30">
@@ -764,7 +764,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="n" s="0">
-        <v>30.578998747395115</v>
+        <v>38.63292819991908</v>
       </c>
     </row>
     <row r="31">
@@ -772,7 +772,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="n" s="0">
-        <v>58.37976050330329</v>
+        <v>19.740318025348625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>